<commit_message>
Added Header and Favicon
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Documents/UCI/Organizations/Delta_Sigma_Pi/Director_of_Technology/dspuci-website-gatsby/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyenokida/Projects/dspuci-website-gatsby/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8793F205-F668-7743-8F75-FE99324539D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DE826F-3812-6343-9B75-6AF09012F9FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14620" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internships 2019" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="308">
   <si>
     <t>Name</t>
   </si>
@@ -936,6 +936,27 @@
   </si>
   <si>
     <t>Chief Executive Officer</t>
+  </si>
+  <si>
+    <t>Finance &amp; Accounting</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>Marketing &amp; Sales</t>
+  </si>
+  <si>
+    <t>Technology &amp; PM</t>
+  </si>
+  <si>
+    <t>Human Resources &amp; Administration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consulting </t>
+  </si>
+  <si>
+    <t>Technology and PM</t>
   </si>
 </sst>
 </file>
@@ -1215,15 +1236,15 @@
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="49.83203125" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" customWidth="1"/>
     <col min="4" max="4" width="19.5" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
   </cols>
@@ -1849,6 +1870,9 @@
       </c>
       <c r="C37" s="1" t="s">
         <v>153</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>18</v>
@@ -2442,15 +2466,16 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="36.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
@@ -2464,6 +2489,9 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2478,6 +2506,9 @@
         <v>249</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2492,6 +2523,9 @@
         <v>219</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>250</v>
       </c>
     </row>
@@ -2506,6 +2540,9 @@
         <v>251</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2520,6 +2557,9 @@
         <v>110</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2534,6 +2574,9 @@
         <v>254</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2548,6 +2591,9 @@
         <v>256</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2562,6 +2608,9 @@
         <v>258</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2576,6 +2625,9 @@
         <v>59</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2589,7 +2641,10 @@
       <c r="C10" t="s">
         <v>260</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2603,7 +2658,10 @@
       <c r="C11" t="s">
         <v>261</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E11" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2617,7 +2675,10 @@
       <c r="C12" t="s">
         <v>233</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E12" t="s">
         <v>234</v>
       </c>
       <c r="G12" s="4"/>
@@ -2633,7 +2694,10 @@
       <c r="C13" t="s">
         <v>187</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E13" t="s">
         <v>188</v>
       </c>
       <c r="G13" s="4"/>
@@ -2649,7 +2713,10 @@
       <c r="C14" t="s">
         <v>263</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
         <v>264</v>
       </c>
       <c r="G14" s="4"/>
@@ -2665,7 +2732,10 @@
       <c r="C15" t="s">
         <v>224</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E15" t="s">
         <v>225</v>
       </c>
       <c r="G15" s="4"/>
@@ -2681,7 +2751,10 @@
       <c r="C16" t="s">
         <v>266</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E16" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="4"/>
@@ -2697,7 +2770,10 @@
       <c r="C17" t="s">
         <v>267</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E17" t="s">
         <v>268</v>
       </c>
       <c r="G17" s="4"/>
@@ -2713,7 +2789,10 @@
       <c r="C18" t="s">
         <v>270</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="E18" t="s">
         <v>46</v>
       </c>
       <c r="G18" s="4"/>
@@ -2729,7 +2808,10 @@
       <c r="C19" t="s">
         <v>71</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E19" t="s">
         <v>29</v>
       </c>
       <c r="G19" s="4"/>
@@ -2745,7 +2827,10 @@
       <c r="C20" t="s">
         <v>221</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E20" t="s">
         <v>222</v>
       </c>
       <c r="G20" s="4"/>
@@ -2761,7 +2846,10 @@
       <c r="C21" t="s">
         <v>272</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="E21" t="s">
         <v>172</v>
       </c>
       <c r="G21" s="4"/>
@@ -2777,7 +2865,10 @@
       <c r="C22" t="s">
         <v>289</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E22" t="s">
         <v>287</v>
       </c>
       <c r="G22" s="4"/>
@@ -2793,7 +2884,10 @@
       <c r="C23" t="s">
         <v>273</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E23" t="s">
         <v>274</v>
       </c>
       <c r="G23" s="4"/>
@@ -2809,7 +2903,10 @@
       <c r="C24" t="s">
         <v>224</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E24" t="s">
         <v>225</v>
       </c>
       <c r="G24" s="4"/>
@@ -2825,7 +2922,10 @@
       <c r="C25" t="s">
         <v>288</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E25" t="s">
         <v>287</v>
       </c>
       <c r="G25" s="4"/>
@@ -2841,7 +2941,10 @@
       <c r="C26" t="s">
         <v>277</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E26" t="s">
         <v>11</v>
       </c>
       <c r="G26" s="4"/>
@@ -2857,7 +2960,10 @@
       <c r="C27" t="s">
         <v>59</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E27" t="s">
         <v>72</v>
       </c>
       <c r="G27" s="4"/>
@@ -2873,7 +2979,10 @@
       <c r="C28" t="s">
         <v>290</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E28" t="s">
         <v>287</v>
       </c>
       <c r="G28" s="4"/>
@@ -2889,7 +2998,10 @@
       <c r="C29" t="s">
         <v>280</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E29" t="s">
         <v>7</v>
       </c>
       <c r="G29" s="4"/>
@@ -2905,7 +3017,10 @@
       <c r="C30" t="s">
         <v>282</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="E30" t="s">
         <v>18</v>
       </c>
       <c r="G30" s="4"/>
@@ -2921,7 +3036,10 @@
       <c r="C31" t="s">
         <v>221</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E31" t="s">
         <v>222</v>
       </c>
       <c r="G31" s="4"/>
@@ -2937,7 +3055,10 @@
       <c r="C32" t="s">
         <v>110</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E32" t="s">
         <v>284</v>
       </c>
       <c r="G32" s="4"/>
@@ -2953,7 +3074,10 @@
       <c r="C33" t="s">
         <v>285</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E33" t="s">
         <v>130</v>
       </c>
       <c r="G33" s="4"/>
@@ -2969,7 +3093,10 @@
       <c r="C34" t="s">
         <v>286</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E34" t="s">
         <v>287</v>
       </c>
       <c r="G34" s="4"/>
@@ -2985,7 +3112,10 @@
       <c r="C35" t="s">
         <v>71</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E35" t="s">
         <v>29</v>
       </c>
       <c r="G35" s="4"/>
@@ -3001,7 +3131,10 @@
       <c r="C36" t="s">
         <v>78</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E36" t="s">
         <v>80</v>
       </c>
       <c r="G36" s="4"/>
@@ -3058,11 +3191,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3070,9 +3203,10 @@
     <col min="2" max="2" width="40.33203125" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3083,10 +3217,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -3097,10 +3234,13 @@
         <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>301</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -3111,10 +3251,13 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>39</v>
       </c>
@@ -3125,10 +3268,13 @@
         <v>292</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>106</v>
       </c>
@@ -3139,10 +3285,13 @@
         <v>33</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>301</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
@@ -3153,10 +3302,13 @@
         <v>219</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -3167,10 +3319,13 @@
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>98</v>
       </c>
@@ -3181,10 +3336,13 @@
         <v>100</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>306</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>114</v>
       </c>
@@ -3195,10 +3353,13 @@
         <v>296</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>118</v>
       </c>
@@ -3209,10 +3370,13 @@
         <v>229</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>171</v>
       </c>
@@ -3223,10 +3387,13 @@
         <v>168</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>166</v>
       </c>
@@ -3237,10 +3404,13 @@
         <v>168</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>177</v>
       </c>
@@ -3251,10 +3421,13 @@
         <v>45</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>178</v>
       </c>
@@ -3265,10 +3438,13 @@
         <v>168</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>182</v>
       </c>
@@ -3279,10 +3455,13 @@
         <v>224</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>298</v>
       </c>
@@ -3293,6 +3472,9 @@
         <v>299</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed fonts, updated careers page info
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyenokida/Projects/dspuci-website-gatsby/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF711442-DD80-194D-BCE9-13C14A3EA196}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE203FEF-615E-2F4B-A6BD-C91679CD8E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4480" yWindow="1100" windowWidth="21160" windowHeight="14300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4480" yWindow="1100" windowWidth="21160" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Time Offers 2020" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="622">
   <si>
     <t>Name</t>
   </si>
@@ -792,9 +792,6 @@
     <t>California Bank &amp; Trust</t>
   </si>
   <si>
-    <t>Corporate and Investmnet Bank Analyst</t>
-  </si>
-  <si>
     <t>New York City, NY</t>
   </si>
   <si>
@@ -1912,6 +1909,9 @@
   </si>
   <si>
     <t>University of California, Irvine</t>
+  </si>
+  <si>
+    <t>Sales and Trading Analyst</t>
   </si>
 </sst>
 </file>
@@ -2204,9 +2204,9 @@
   </sheetPr>
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -2331,36 +2331,36 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="A10" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>250</v>
+        <v>195</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>251</v>
+        <v>196</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>7</v>
@@ -2368,21 +2368,21 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>195</v>
+        <v>621</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>7</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2393,7 +2393,7 @@
         <v>145</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>143</v>
@@ -2407,7 +2407,7 @@
         <v>141</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>143</v>
@@ -2471,7 +2471,7 @@
         <v>152</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>143</v>
@@ -2534,7 +2534,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -2542,27 +2542,27 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>454</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>455</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>7</v>
@@ -2570,7 +2570,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>35</v>
@@ -2584,7 +2584,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>35</v>
@@ -2598,13 +2598,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>456</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>457</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>17</v>
@@ -2612,10 +2612,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>226</v>
@@ -2626,13 +2626,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>459</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>460</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>17</v>
@@ -2640,7 +2640,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>35</v>
@@ -2654,7 +2654,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -2662,21 +2662,21 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>462</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2684,13 +2684,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>17</v>
@@ -2698,13 +2698,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>104</v>
@@ -2712,13 +2712,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>17</v>
@@ -2726,13 +2726,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>466</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>467</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>17</v>
@@ -2740,13 +2740,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>468</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>469</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>17</v>
@@ -2754,13 +2754,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>17</v>
@@ -2768,13 +2768,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>470</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>471</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>17</v>
@@ -2782,13 +2782,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>472</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>473</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
@@ -2796,13 +2796,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>17</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2818,13 +2818,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>475</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>476</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>201</v>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -2840,13 +2840,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>25</v>
@@ -2854,13 +2854,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>17</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>479</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>480</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>17</v>
@@ -2933,21 +2933,21 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>494</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -2955,7 +2955,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>14</v>
@@ -2969,10 +2969,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>482</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>483</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>29</v>
@@ -2983,7 +2983,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -2991,13 +2991,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>484</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>485</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>486</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -3005,13 +3005,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>488</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>489</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>192</v>
@@ -3019,7 +3019,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -3027,13 +3027,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>490</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>491</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>10</v>
@@ -3076,7 +3076,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3084,7 +3084,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>35</v>
@@ -3098,27 +3098,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>497</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>500</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>501</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>17</v>
@@ -3126,7 +3126,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>52</v>
@@ -3140,13 +3140,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>182</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>17</v>
@@ -3154,13 +3154,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>504</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>505</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -3168,13 +3168,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>508</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>17</v>
@@ -3182,13 +3182,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>456</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>457</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>17</v>
@@ -3196,27 +3196,27 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>510</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>511</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>17</v>
@@ -3224,21 +3224,21 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>513</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -3246,13 +3246,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>17</v>
@@ -3260,13 +3260,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>516</v>
-      </c>
       <c r="C16" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>17</v>
@@ -3274,27 +3274,27 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>518</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>17</v>
@@ -3302,27 +3302,27 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>520</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>521</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>522</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>423</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>424</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>17</v>
@@ -3330,7 +3330,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -3338,13 +3338,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>153</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>17</v>
@@ -3352,13 +3352,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>527</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>528</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>17</v>
@@ -3366,35 +3366,35 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>531</v>
-      </c>
       <c r="D24" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>153</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -3402,27 +3402,27 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>533</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>128</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>69</v>
@@ -3473,10 +3473,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>546</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>547</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>23</v>
@@ -3487,10 +3487,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>548</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>549</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>23</v>
@@ -3501,7 +3501,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -3509,13 +3509,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>537</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>538</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>539</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>10</v>
@@ -3523,21 +3523,21 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>13</v>
@@ -3551,24 +3551,24 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>542</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>543</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>15</v>
@@ -3579,7 +3579,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -3587,10 +3587,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>550</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>551</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>196</v>
@@ -3601,13 +3601,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>552</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>553</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>554</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -3623,13 +3623,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>555</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>556</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>17</v>
@@ -3637,13 +3637,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>557</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>558</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>559</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>244</v>
@@ -3694,13 +3694,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>578</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>579</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>580</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>17</v>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -3716,13 +3716,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>17</v>
@@ -3730,13 +3730,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>17</v>
@@ -3744,13 +3744,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>17</v>
@@ -3758,13 +3758,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -3772,10 +3772,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>15</v>
@@ -3786,27 +3786,27 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>564</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>500</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>501</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>17</v>
@@ -3814,10 +3814,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>53</v>
@@ -3828,13 +3828,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
+        <v>567</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>568</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>569</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>570</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -3842,27 +3842,27 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
+        <v>570</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>571</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>572</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>574</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>575</v>
-      </c>
       <c r="C15" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>17</v>
@@ -3870,13 +3870,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>576</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>577</v>
-      </c>
       <c r="C16" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>17</v>
@@ -3884,7 +3884,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -3892,27 +3892,27 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>581</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>582</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>583</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
+        <v>584</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>585</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>586</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>587</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>17</v>
@@ -3920,7 +3920,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -3928,13 +3928,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
@@ -3942,13 +3942,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>587</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>588</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>589</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>17</v>
@@ -3956,13 +3956,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>590</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>591</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>592</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>40</v>
@@ -3970,13 +3970,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>118</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>17</v>
@@ -3984,13 +3984,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
+        <v>594</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>595</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>596</v>
-      </c>
       <c r="C25" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>17</v>
@@ -3998,27 +3998,27 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>597</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>598</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>600</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>601</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>602</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>17</v>
@@ -4026,13 +4026,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>603</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>604</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>605</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>10</v>
@@ -4040,21 +4040,21 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>606</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>597</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>607</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -4062,13 +4062,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>17</v>
@@ -4076,13 +4076,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>610</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>611</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>17</v>
@@ -4090,7 +4090,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -4098,13 +4098,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>613</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>614</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>17</v>
@@ -4112,13 +4112,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>17</v>
@@ -4126,13 +4126,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>616</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>617</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>69</v>
@@ -4140,13 +4140,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>618</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>619</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>17</v>
@@ -4154,13 +4154,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>620</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>621</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>17</v>
@@ -4175,7 +4175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B663391-D25B-0045-851E-8A0BB00A0B0A}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
@@ -4215,7 +4215,7 @@
         <v>79</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>223</v>
@@ -4226,7 +4226,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -4243,7 +4243,7 @@
         <v>186</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
@@ -4265,7 +4265,7 @@
         <v>184</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>218</v>
@@ -4355,7 +4355,7 @@
         <v>58</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>92</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -4384,7 +4384,7 @@
         <v>219</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>17</v>
@@ -4429,7 +4429,7 @@
         <v>212</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>240</v>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -4522,7 +4522,7 @@
         <v>97</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>244</v>
@@ -4600,7 +4600,7 @@
         <v>237</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>244</v>
@@ -4608,7 +4608,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4658,7 +4658,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -4672,7 +4672,7 @@
         <v>193</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>155</v>
@@ -4857,7 +4857,7 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -4893,7 +4893,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -4915,7 +4915,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -4965,7 +4965,7 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -4987,7 +4987,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -5087,7 +5087,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -5263,7 +5263,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -5327,7 +5327,7 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -5517,7 +5517,7 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -5539,7 +5539,7 @@
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -5716,10 +5716,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D48177-9EF2-1D45-80EE-751A8F12EE03}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5746,7 +5746,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -5754,7 +5754,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>13</v>
@@ -5768,10 +5768,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>273</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>50</v>
@@ -5782,10 +5782,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>275</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>29</v>
@@ -5796,13 +5796,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>277</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>278</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>17</v>
@@ -5810,10 +5810,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>279</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>280</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>50</v>
@@ -5824,7 +5824,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -5832,13 +5832,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>283</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>17</v>
@@ -5846,7 +5846,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -5854,13 +5854,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>118</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>17</v>
@@ -5868,13 +5868,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>287</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>288</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>10</v>
@@ -5882,13 +5882,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>290</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>291</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>10</v>
@@ -5896,13 +5896,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>293</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>294</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>17</v>
@@ -5910,13 +5910,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>296</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>297</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>7</v>
@@ -5924,43 +5924,43 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+        <v>256</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>194</v>
+        <v>302</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>143</v>
+        <v>303</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>144</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>194</v>
+        <v>305</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>301</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -5968,51 +5968,43 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>303</v>
+        <v>194</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>304</v>
+        <v>143</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>233</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>306</v>
+        <v>194</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>17</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="3" t="s">
+      <c r="A22" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -6052,7 +6044,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -6080,10 +6072,10 @@
         <v>52</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -6091,7 +6083,7 @@
         <v>90</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>92</v>
@@ -6105,10 +6097,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>315</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>316</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>10</v>
@@ -6136,7 +6128,7 @@
         <v>86</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -6147,7 +6139,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>9</v>
@@ -6164,10 +6156,10 @@
         <v>52</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>319</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
@@ -6175,10 +6167,10 @@
         <v>26</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>321</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>322</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>7</v>
@@ -6186,7 +6178,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -6197,10 +6189,10 @@
         <v>79</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>323</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>324</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>7</v>
@@ -6208,7 +6200,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -6219,10 +6211,10 @@
         <v>174</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>325</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>326</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>17</v>
@@ -6247,10 +6239,10 @@
         <v>47</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>327</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>328</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>17</v>
@@ -6261,10 +6253,10 @@
         <v>120</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>329</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>330</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>17</v>
@@ -6275,7 +6267,7 @@
         <v>41</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>113</v>
@@ -6292,7 +6284,7 @@
         <v>137</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>17</v>
@@ -6303,10 +6295,10 @@
         <v>103</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
@@ -6317,18 +6309,18 @@
         <v>54</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6339,7 +6331,7 @@
         <v>57</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>50</v>
@@ -6353,10 +6345,10 @@
         <v>145</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>337</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>338</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>99</v>
@@ -6364,13 +6356,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>340</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>341</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>126</v>
@@ -6381,10 +6373,10 @@
         <v>147</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>342</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>343</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>107</v>
@@ -6395,13 +6387,13 @@
         <v>152</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>345</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
@@ -6409,18 +6401,18 @@
         <v>21</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>348</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -6428,13 +6420,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>351</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>352</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>17</v>
@@ -6442,7 +6434,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -6453,10 +6445,10 @@
         <v>37</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>353</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>354</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>17</v>
@@ -6464,13 +6456,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>356</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>357</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>10</v>
@@ -6513,7 +6505,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -6521,13 +6513,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>359</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>360</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>7</v>
@@ -6535,13 +6527,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>7</v>
@@ -6549,24 +6541,24 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>365</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>29</v>
@@ -6577,10 +6569,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>368</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>369</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>15</v>
@@ -6591,7 +6583,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -6599,27 +6591,27 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>372</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>375</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>376</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>126</v>
@@ -6627,13 +6619,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>378</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>379</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>17</v>
@@ -6641,7 +6633,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -6649,27 +6641,27 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>382</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>384</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>385</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>17</v>
@@ -6677,7 +6669,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -6685,13 +6677,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>387</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>388</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>17</v>
@@ -6699,7 +6691,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -6707,13 +6699,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>390</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>391</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>17</v>
@@ -6756,7 +6748,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -6764,7 +6756,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>87</v>
@@ -6778,24 +6770,24 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>393</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>50</v>
@@ -6809,10 +6801,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>396</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>397</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>7</v>
@@ -6820,7 +6812,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>86</v>
@@ -6834,13 +6826,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>398</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>399</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -6848,13 +6840,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>17</v>
@@ -6862,10 +6854,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>401</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>402</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>226</v>
@@ -6876,13 +6868,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>404</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>405</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>17</v>
@@ -6893,7 +6885,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>226</v>
@@ -6907,10 +6899,10 @@
         <v>44</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -6918,10 +6910,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>50</v>
@@ -6932,7 +6924,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -6943,10 +6935,10 @@
         <v>174</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>408</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>409</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>7</v>
@@ -6954,27 +6946,27 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>409</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>410</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>411</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>412</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>17</v>
@@ -6982,7 +6974,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -7004,13 +6996,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
@@ -7021,10 +7013,10 @@
         <v>47</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>327</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>328</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>17</v>
@@ -7032,10 +7024,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>50</v>
@@ -7052,7 +7044,7 @@
         <v>137</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>17</v>
@@ -7060,27 +7052,27 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>417</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>137</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>126</v>
@@ -7088,13 +7080,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>17</v>
@@ -7102,13 +7094,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>166</v>
@@ -7116,13 +7108,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>17</v>
@@ -7133,10 +7125,10 @@
         <v>21</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>423</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>424</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>17</v>
@@ -7144,13 +7136,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>425</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>426</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>427</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>10</v>
@@ -7158,7 +7150,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -7166,10 +7158,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>143</v>
@@ -7180,21 +7172,21 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>153</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -7202,27 +7194,27 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>17</v>
@@ -7230,7 +7222,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -7238,13 +7230,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>432</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>433</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>25</v>
@@ -7295,10 +7287,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>442</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>443</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>23</v>
@@ -7309,7 +7301,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -7317,7 +7309,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
@@ -7331,10 +7323,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>29</v>
@@ -7345,13 +7337,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>436</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>437</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>17</v>
@@ -7359,10 +7351,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>15</v>
@@ -7373,21 +7365,21 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>440</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>441</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -7395,10 +7387,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>67</v>
@@ -7409,13 +7401,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>445</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>446</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>447</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>17</v>
@@ -7423,13 +7415,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>449</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>450</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -7437,13 +7429,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>451</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>452</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Fixed 2018 career changes
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyenokida/Projects/dspuci-website-gatsby/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4CB9E4-5BD4-C240-AB24-E6FA5FA0352A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D621CA4F-8933-CE4D-AC29-ADEF212707D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="2240" windowWidth="21160" windowHeight="14300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Time Offers 2021" sheetId="15" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="631">
   <si>
     <t>Name</t>
   </si>
@@ -941,9 +941,6 @@
     <t>Sequoia</t>
   </si>
   <si>
-    <t>Technical</t>
-  </si>
-  <si>
     <t>Nathan Wang</t>
   </si>
   <si>
@@ -1941,6 +1938,9 @@
   </si>
   <si>
     <t>2021 CADP Summer Analyst</t>
+  </si>
+  <si>
+    <t>Product Marketing Manager</t>
   </si>
 </sst>
 </file>
@@ -2228,10 +2228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3CD6D6-8A13-7342-A149-99232F890266}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="A1:D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2266,82 +2266,98 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>623</v>
+      <c r="D3" s="1" t="s">
+        <v>622</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>626</v>
+        <v>92</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>211</v>
+        <v>79</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>624</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>92</v>
+        <v>625</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>252</v>
+        <v>211</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>622</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
@@ -2350,7 +2366,7 @@
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="6"/>
+      <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -2386,7 +2402,7 @@
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="3"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2405,6 +2421,24 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2465,16 +2499,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>392</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -2482,7 +2516,7 @@
         <v>271</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>50</v>
@@ -2496,10 +2530,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>395</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>396</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>7</v>
@@ -2521,13 +2555,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>397</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>398</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -2538,7 +2572,7 @@
         <v>275</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>277</v>
@@ -2549,10 +2583,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>400</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>401</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>226</v>
@@ -2563,13 +2597,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>403</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>404</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>17</v>
@@ -2580,7 +2614,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>226</v>
@@ -2594,7 +2628,7 @@
         <v>44</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>262</v>
@@ -2608,7 +2642,7 @@
         <v>278</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>50</v>
@@ -2630,10 +2664,10 @@
         <v>174</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>407</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>408</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>7</v>
@@ -2641,13 +2675,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>407</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>408</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>258</v>
@@ -2655,13 +2689,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>410</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>411</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>17</v>
@@ -2691,13 +2725,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
@@ -2708,10 +2742,10 @@
         <v>47</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>326</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>327</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>17</v>
@@ -2739,7 +2773,7 @@
         <v>137</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>17</v>
@@ -2747,21 +2781,21 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>416</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>137</v>
@@ -2775,13 +2809,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>17</v>
@@ -2795,7 +2829,7 @@
         <v>97</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>166</v>
@@ -2803,13 +2837,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>17</v>
@@ -2820,10 +2854,10 @@
         <v>21</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>422</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>423</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>17</v>
@@ -2831,13 +2865,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>425</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>426</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>10</v>
@@ -2853,10 +2887,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>143</v>
@@ -2867,7 +2901,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>153</v>
@@ -2876,7 +2910,7 @@
         <v>290</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
@@ -2889,27 +2923,27 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>267</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>17</v>
@@ -2917,7 +2951,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -2925,13 +2959,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>431</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>432</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>25</v>
@@ -2982,10 +3016,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>441</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>442</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>23</v>
@@ -3004,7 +3038,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
@@ -3018,7 +3052,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>274</v>
@@ -3032,13 +3066,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>435</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>436</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>17</v>
@@ -3046,10 +3080,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>15</v>
@@ -3060,13 +3094,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>439</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>440</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>258</v>
@@ -3082,10 +3116,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>67</v>
@@ -3096,13 +3130,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>445</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>446</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>17</v>
@@ -3110,13 +3144,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>447</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>448</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>449</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -3124,13 +3158,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>295</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>10</v>
@@ -3181,27 +3215,27 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>453</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>454</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>7</v>
@@ -3209,7 +3243,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>35</v>
@@ -3223,7 +3257,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>35</v>
@@ -3237,13 +3271,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>455</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>456</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>17</v>
@@ -3254,7 +3288,7 @@
         <v>280</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>226</v>
@@ -3265,13 +3299,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>458</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>459</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>17</v>
@@ -3279,7 +3313,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>35</v>
@@ -3304,10 +3338,10 @@
         <v>278</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>460</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>461</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>258</v>
@@ -3323,13 +3357,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>17</v>
@@ -3337,13 +3371,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>104</v>
@@ -3357,7 +3391,7 @@
         <v>97</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>17</v>
@@ -3365,13 +3399,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>465</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>466</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>17</v>
@@ -3379,13 +3413,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>467</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>468</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>17</v>
@@ -3399,7 +3433,7 @@
         <v>97</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>17</v>
@@ -3407,13 +3441,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>469</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>470</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>17</v>
@@ -3424,10 +3458,10 @@
         <v>294</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>471</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>472</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
@@ -3435,13 +3469,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>17</v>
@@ -3457,13 +3491,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>474</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>475</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>201</v>
@@ -3479,13 +3513,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>267</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>25</v>
@@ -3499,7 +3533,7 @@
         <v>266</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>17</v>
@@ -3507,7 +3541,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -3515,13 +3549,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>478</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>479</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>17</v>
@@ -3572,16 +3606,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>493</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -3594,7 +3628,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>14</v>
@@ -3608,10 +3642,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>481</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>482</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>29</v>
@@ -3630,13 +3664,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>484</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>485</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -3644,13 +3678,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>487</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>488</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>192</v>
@@ -3666,13 +3700,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>10</v>
@@ -3723,7 +3757,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>35</v>
@@ -3737,27 +3771,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>496</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>499</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>500</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>17</v>
@@ -3765,7 +3799,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>52</v>
@@ -3779,13 +3813,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>182</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>17</v>
@@ -3793,13 +3827,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>503</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>504</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -3807,13 +3841,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>505</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>506</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>507</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>17</v>
@@ -3821,13 +3855,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>455</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>456</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>17</v>
@@ -3835,13 +3869,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>509</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>510</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>258</v>
@@ -3849,13 +3883,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>17</v>
@@ -3863,16 +3897,16 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>512</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
@@ -3885,13 +3919,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>17</v>
@@ -3899,13 +3933,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>514</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>515</v>
-      </c>
       <c r="C16" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>17</v>
@@ -3913,27 +3947,27 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>517</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>17</v>
@@ -3941,27 +3975,27 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>519</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>520</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>521</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>422</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>423</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>17</v>
@@ -3977,13 +4011,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>153</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>17</v>
@@ -3991,13 +4025,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>526</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>527</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>17</v>
@@ -4005,35 +4039,35 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>530</v>
-      </c>
       <c r="D24" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>153</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -4041,27 +4075,27 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>532</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>128</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>69</v>
@@ -4112,10 +4146,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>545</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>546</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>23</v>
@@ -4126,10 +4160,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>547</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>548</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>23</v>
@@ -4148,13 +4182,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>537</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>538</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>10</v>
@@ -4162,10 +4196,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>14</v>
@@ -4176,7 +4210,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>13</v>
@@ -4190,21 +4224,21 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>541</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>542</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>274</v>
@@ -4226,10 +4260,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>549</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>550</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>196</v>
@@ -4240,13 +4274,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>551</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>552</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>553</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -4262,13 +4296,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>554</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>555</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>17</v>
@@ -4276,13 +4310,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>556</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>557</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>558</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>244</v>
@@ -4333,13 +4367,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>577</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>578</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>579</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>17</v>
@@ -4355,13 +4389,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>17</v>
@@ -4369,13 +4403,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>17</v>
@@ -4383,13 +4417,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>17</v>
@@ -4397,13 +4431,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -4411,10 +4445,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>15</v>
@@ -4425,27 +4459,27 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>563</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>499</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>500</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>17</v>
@@ -4453,10 +4487,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>53</v>
@@ -4467,13 +4501,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>567</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>568</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>569</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -4481,27 +4515,27 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>570</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>571</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>277</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>573</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>574</v>
-      </c>
       <c r="C15" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>17</v>
@@ -4509,13 +4543,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>575</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>576</v>
-      </c>
       <c r="C16" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>17</v>
@@ -4531,27 +4565,27 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>580</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>581</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>582</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
+        <v>583</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>584</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>585</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>586</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>17</v>
@@ -4567,13 +4601,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
@@ -4581,13 +4615,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>586</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>587</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>588</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>17</v>
@@ -4595,13 +4629,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
+        <v>588</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>589</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>590</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>591</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>40</v>
@@ -4609,13 +4643,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>118</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>17</v>
@@ -4623,13 +4657,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>594</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>595</v>
-      </c>
       <c r="C25" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>17</v>
@@ -4637,27 +4671,27 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>596</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>597</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>600</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>601</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>17</v>
@@ -4665,13 +4699,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>602</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>603</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>604</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>10</v>
@@ -4679,16 +4713,16 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>605</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>596</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>606</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
@@ -4701,13 +4735,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>266</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>17</v>
@@ -4715,13 +4749,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>609</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>610</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>17</v>
@@ -4729,7 +4763,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -4737,13 +4771,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>612</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>613</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>17</v>
@@ -4751,13 +4785,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>17</v>
@@ -4765,13 +4799,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>615</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>616</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>69</v>
@@ -4779,13 +4813,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>617</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>618</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>17</v>
@@ -4793,13 +4827,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>619</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>620</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>17</v>
@@ -4814,7 +4848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D299C4D8-108C-C347-A079-14D1CC67BEF2}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -4853,13 +4887,13 @@
         <v>178</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -4875,13 +4909,13 @@
         <v>205</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>628</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>629</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -4889,13 +4923,13 @@
         <v>138</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>186</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
@@ -4917,7 +4951,7 @@
         <v>143</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
@@ -4964,7 +4998,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="A1:D22"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5093,7 +5127,7 @@
         <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>186</v>
@@ -6808,7 +6842,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7021,13 +7055,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>302</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>303</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>233</v>
@@ -7035,13 +7069,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>306</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>17</v>
@@ -7057,7 +7091,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>194</v>
@@ -7071,7 +7105,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>194</v>
@@ -7080,18 +7114,18 @@
         <v>290</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>309</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>310</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>10</v>
@@ -7104,15 +7138,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B2E965-35C6-B34F-B96B-27E9F0AE48DD}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="26" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="46.5" customWidth="1"/>
     <col min="3" max="3" width="31.5" customWidth="1"/>
     <col min="4" max="4" width="36.83203125" customWidth="1"/>
   </cols>
@@ -7161,10 +7196,10 @@
         <v>52</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>311</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -7172,7 +7207,7 @@
         <v>90</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>92</v>
@@ -7186,10 +7221,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>315</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>10</v>
@@ -7217,7 +7252,7 @@
         <v>86</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -7228,7 +7263,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>9</v>
@@ -7245,10 +7280,10 @@
         <v>52</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>318</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
@@ -7256,10 +7291,10 @@
         <v>26</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>321</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>7</v>
@@ -7278,10 +7313,10 @@
         <v>79</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>322</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>323</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>7</v>
@@ -7300,10 +7335,10 @@
         <v>174</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>324</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>325</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>17</v>
@@ -7328,10 +7363,10 @@
         <v>47</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>326</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>327</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>17</v>
@@ -7342,10 +7377,10 @@
         <v>120</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>328</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>329</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>17</v>
@@ -7356,7 +7391,7 @@
         <v>41</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>113</v>
@@ -7373,7 +7408,7 @@
         <v>137</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>17</v>
@@ -7384,10 +7419,10 @@
         <v>103</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
@@ -7398,163 +7433,155 @@
         <v>54</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+        <v>256</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>57</v>
+        <v>348</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>335</v>
+        <v>349</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>50</v>
+        <v>350</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>99</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>338</v>
+        <v>37</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>339</v>
+        <v>351</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>340</v>
+        <v>352</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>126</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>147</v>
+        <v>353</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>342</v>
+        <v>355</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>107</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
-        <v>152</v>
+        <v>57</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>344</v>
+        <v>50</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>345</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>348</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+        <v>337</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
-        <v>349</v>
+        <v>147</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
+        <v>152</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>10</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -7602,13 +7629,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>358</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>359</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>7</v>
@@ -7616,13 +7643,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>7</v>
@@ -7630,21 +7657,21 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>364</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>274</v>
@@ -7658,10 +7685,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>367</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>368</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>15</v>
@@ -7680,27 +7707,27 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>371</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>374</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>375</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>126</v>
@@ -7708,13 +7735,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>377</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>378</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>17</v>
@@ -7730,27 +7757,27 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>381</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>382</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>383</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>384</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>17</v>
@@ -7766,13 +7793,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>386</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>387</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>17</v>
@@ -7780,7 +7807,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -7788,13 +7815,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>389</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>390</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
reverted changes from google sheets back to previous excel sheets
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyenokida/Projects/dspuci-website-gatsby/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D621CA4F-8933-CE4D-AC29-ADEF212707D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CD9C89-DF8F-1D43-BA88-C133F9792924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39440" yWindow="-5660" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Time Offers 2021" sheetId="15" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="681">
   <si>
     <t>Name</t>
   </si>
@@ -1931,23 +1931,173 @@
     <t>Consulting Intern</t>
   </si>
   <si>
-    <t>Rotational Research Intern</t>
-  </si>
-  <si>
-    <t>Green Street Advisors</t>
-  </si>
-  <si>
     <t>2021 CADP Summer Analyst</t>
   </si>
   <si>
     <t>Product Marketing Manager</t>
+  </si>
+  <si>
+    <t>Tommy Truong</t>
+  </si>
+  <si>
+    <t>Summer Research Consulting Intern</t>
+  </si>
+  <si>
+    <t>Linda S. Congleton &amp; Associates</t>
+  </si>
+  <si>
+    <t>Sophomore Investment Banking Summer Analyst</t>
+  </si>
+  <si>
+    <t>Deutsche Bank</t>
+  </si>
+  <si>
+    <t>Aarti Vellimedu</t>
+  </si>
+  <si>
+    <t>2021 Summer Financial Analyst - Capital Finance</t>
+  </si>
+  <si>
+    <t>Portfolio Analyst Intern</t>
+  </si>
+  <si>
+    <t>NationalGrid</t>
+  </si>
+  <si>
+    <t>Private Equity Summer Analyst</t>
+  </si>
+  <si>
+    <t>Everstone Group</t>
+  </si>
+  <si>
+    <t>Darren Han</t>
+  </si>
+  <si>
+    <t>Private Equity Investment Intern</t>
+  </si>
+  <si>
+    <t>Pathway Capital Management</t>
+  </si>
+  <si>
+    <t>Cyber Risk Advisory Intern</t>
+  </si>
+  <si>
+    <t>Alex Pham</t>
+  </si>
+  <si>
+    <t>Project Management Intern</t>
+  </si>
+  <si>
+    <t>AT&amp;T</t>
+  </si>
+  <si>
+    <t>Beyond Limits AI</t>
+  </si>
+  <si>
+    <t>Brennen Wong</t>
+  </si>
+  <si>
+    <t>Systems Developer Intern</t>
+  </si>
+  <si>
+    <t>MarketMAPS</t>
+  </si>
+  <si>
+    <t>Sean Devine</t>
+  </si>
+  <si>
+    <t>Data Science Intern</t>
+  </si>
+  <si>
+    <t>IQVIA</t>
+  </si>
+  <si>
+    <t>Business Strategy &amp; Marketing Intern</t>
+  </si>
+  <si>
+    <t>Autodesk</t>
+  </si>
+  <si>
+    <t>Sales Development Representative</t>
+  </si>
+  <si>
+    <t>Slack Inc.</t>
+  </si>
+  <si>
+    <t>Sales Intern - Global Business Solutions</t>
+  </si>
+  <si>
+    <t>Consumer Product Retail Development Intern</t>
+  </si>
+  <si>
+    <t>NBCUniversal Media</t>
+  </si>
+  <si>
+    <t>Jessie Yang</t>
+  </si>
+  <si>
+    <t>Sales Analytics &amp; Sales Operations Intern</t>
+  </si>
+  <si>
+    <t>VEVO</t>
+  </si>
+  <si>
+    <t>Yeseo Han</t>
+  </si>
+  <si>
+    <t>Virtual HR &amp; Company</t>
+  </si>
+  <si>
+    <t>Kevin Cao</t>
+  </si>
+  <si>
+    <t>Social Media Manager Intern</t>
+  </si>
+  <si>
+    <t>OPTIS Group Holdings</t>
+  </si>
+  <si>
+    <t>Kelsie Kim</t>
+  </si>
+  <si>
+    <t>Marketing Administrative Assistant</t>
+  </si>
+  <si>
+    <t>DPM Link</t>
+  </si>
+  <si>
+    <t>University Talent Experience Intern</t>
+  </si>
+  <si>
+    <t>The Estée Lauder Companies</t>
+  </si>
+  <si>
+    <t>Amanda Nguyen</t>
+  </si>
+  <si>
+    <t>Business Development Intern</t>
+  </si>
+  <si>
+    <t>Oppti</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
+  </si>
+  <si>
+    <t>Acquisitions Analyst Intern</t>
+  </si>
+  <si>
+    <t>Next Wave Investors</t>
+  </si>
+  <si>
+    <t>Program Manager</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1983,6 +2133,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2004,7 +2161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -2013,6 +2170,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2230,8 +2388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3CD6D6-8A13-7342-A149-99232F890266}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2243,26 +2401,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
@@ -2274,7 +2432,7 @@
       <c r="C3" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>622</v>
       </c>
     </row>
@@ -2321,7 +2479,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="8" t="s">
         <v>254</v>
       </c>
       <c r="B7" s="3"/>
@@ -2333,43 +2491,58 @@
         <v>108</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="3" t="s">
-        <v>252</v>
-      </c>
+      <c r="A9" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>621</v>
+        <v>680</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="3"/>
+      <c r="A11" s="8" t="s">
+        <v>252</v>
+      </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
@@ -4846,10 +5019,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D299C4D8-108C-C347-A079-14D1CC67BEF2}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4861,26 +5034,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
@@ -4898,91 +5071,449 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>628</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>622</v>
-      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>138</v>
+        <v>205</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>186</v>
+        <v>633</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="6" t="s">
+        <v>640</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="6" t="s">
+        <v>644</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>646</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B19" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36" s="8" t="s">
+        <v>677</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>622</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4998,7 +5529,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5008,29 +5539,31 @@
     <col min="4" max="4" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -5044,7 +5577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>83</v>
       </c>
@@ -5057,16 +5590,17 @@
       <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
         <v>252</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -5079,8 +5613,9 @@
       <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -5093,8 +5628,9 @@
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -5108,7 +5644,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>88</v>
       </c>
@@ -5121,8 +5657,9 @@
       <c r="D9" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>44</v>
       </c>
@@ -5136,15 +5673,15 @@
         <v>248</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="7" t="s">
         <v>254</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>96</v>
       </c>
@@ -5158,7 +5695,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>100</v>
       </c>
@@ -5172,15 +5709,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="7" t="s">
         <v>255</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>145</v>
       </c>
@@ -5193,8 +5731,9 @@
       <c r="D15" s="3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>141</v>
       </c>
@@ -5207,6 +5746,7 @@
       <c r="D16" s="3" t="s">
         <v>144</v>
       </c>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
@@ -5271,6 +5811,7 @@
       <c r="D19" s="3" t="s">
         <v>144</v>
       </c>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
@@ -5285,6 +5826,7 @@
       <c r="D20" s="3" t="s">
         <v>192</v>
       </c>
+      <c r="E20" s="3"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D20">
@@ -5298,9 +5840,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B663391-D25B-0045-851E-8A0BB00A0B0A}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5326,7 +5868,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="3"/>
@@ -5348,7 +5890,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="8" t="s">
         <v>252</v>
       </c>
       <c r="B4" s="3"/>
@@ -5490,7 +6032,7 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="8" t="s">
         <v>256</v>
       </c>
       <c r="B14" s="3"/>
@@ -5564,7 +6106,7 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>254</v>
       </c>
       <c r="B19" s="3"/>
@@ -5730,7 +6272,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="8" t="s">
         <v>253</v>
       </c>
       <c r="B30" s="3"/>
@@ -5780,7 +6322,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="8" t="s">
         <v>255</v>
       </c>
       <c r="B34" s="3"/>

</xml_diff>

<commit_message>
updated letter from president, careers page, featured bros
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyenokida/Projects/dspuci-website-gatsby/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brennenwong/dspuci-website-gatsby/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CD9C89-DF8F-1D43-BA88-C133F9792924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF154866-761C-1E49-B765-73E1C24F1936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39440" yWindow="-5660" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Time Offers 2021" sheetId="15" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="690">
   <si>
     <t>Name</t>
   </si>
@@ -2081,9 +2081,6 @@
     <t>Oppti</t>
   </si>
   <si>
-    <t>Real Estate</t>
-  </si>
-  <si>
     <t>Acquisitions Analyst Intern</t>
   </si>
   <si>
@@ -2091,6 +2088,36 @@
   </si>
   <si>
     <t>Program Manager</t>
+  </si>
+  <si>
+    <t>Lab Manager</t>
+  </si>
+  <si>
+    <t>UCI School of Biological Sciences</t>
+  </si>
+  <si>
+    <t>Media Coordinator</t>
+  </si>
+  <si>
+    <t>Recruitics</t>
+  </si>
+  <si>
+    <t>UX E-Commerce Coordinator</t>
+  </si>
+  <si>
+    <t>Princess Polly</t>
+  </si>
+  <si>
+    <t>Finance Associate</t>
+  </si>
+  <si>
+    <t>Torrey Pines Bank</t>
+  </si>
+  <si>
+    <t>Audit and Assurance Associate</t>
+  </si>
+  <si>
+    <t>Risk and Financial Advisor</t>
   </si>
 </sst>
 </file>
@@ -2386,16 +2413,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3CD6D6-8A13-7342-A149-99232F890266}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="52.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" customWidth="1"/>
     <col min="4" max="4" width="40.33203125" customWidth="1"/>
   </cols>
@@ -2424,7 +2451,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>623</v>
@@ -2438,13 +2465,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>92</v>
+        <v>625</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>622</v>
@@ -2452,142 +2479,192 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>79</v>
+        <v>211</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>625</v>
+        <v>92</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>623</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="A6" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>628</v>
+        <v>689</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>188</v>
+        <v>92</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>680</v>
+        <v>686</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>621</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="A12" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="3"/>
+      <c r="A16" s="8" t="s">
+        <v>253</v>
+      </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="A17" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="6"/>
+      <c r="A18" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="3"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2611,7 +2688,58 @@
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="3"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="6"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5019,10 +5147,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D299C4D8-108C-C347-A079-14D1CC67BEF2}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView zoomScale="180" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5093,13 +5221,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>205</v>
+        <v>634</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>632</v>
+        <v>52</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>633</v>
+        <v>290</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>622</v>
@@ -5107,27 +5235,27 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>138</v>
+        <v>202</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>627</v>
+        <v>638</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>186</v>
+        <v>639</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="3" t="s">
-        <v>634</v>
+      <c r="A8" s="6" t="s">
+        <v>640</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>641</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>290</v>
+        <v>642</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>622</v>
@@ -5148,42 +5276,42 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="6" t="s">
-        <v>210</v>
+      <c r="A10" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>77</v>
+        <v>633</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
-        <v>207</v>
+      <c r="A11" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>405</v>
+        <v>627</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>637</v>
+        <v>186</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="3" t="s">
-        <v>202</v>
+      <c r="A12" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>638</v>
+        <v>405</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>622</v>
@@ -5191,155 +5319,155 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>640</v>
+        <v>210</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>642</v>
+        <v>77</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>643</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="A15" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="6" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
-        <v>644</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="D17" s="6" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>645</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>646</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>622</v>
-      </c>
-    </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>622</v>
-      </c>
+      <c r="A19" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>158</v>
+        <v>203</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>153</v>
+        <v>659</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>647</v>
-      </c>
-      <c r="D20" s="6" t="s">
+        <v>660</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>648</v>
+        <v>136</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>649</v>
+        <v>658</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>650</v>
-      </c>
-      <c r="D21" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>652</v>
+        <v>662</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>653</v>
-      </c>
-      <c r="D22" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>206</v>
+        <v>669</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>654</v>
+        <v>670</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>655</v>
+        <v>671</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>622</v>
@@ -5347,13 +5475,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>124</v>
+        <v>666</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>656</v>
+        <v>667</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>657</v>
+        <v>668</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>622</v>
@@ -5361,13 +5489,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>229</v>
+        <v>657</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>622</v>
@@ -5375,147 +5503,232 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
-        <v>203</v>
+        <v>664</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>659</v>
+        <v>325</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>660</v>
+        <v>665</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="3" t="s">
-        <v>661</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>663</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>622</v>
-      </c>
+      <c r="A28" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="3" t="s">
-        <v>664</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>665</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="A29" s="6" t="s">
+        <v>644</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
-        <v>666</v>
+        <v>648</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>667</v>
+        <v>649</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="D30" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="3" t="s">
-        <v>669</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>670</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>671</v>
-      </c>
-      <c r="D31" s="3" t="s">
+      <c r="A31" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>646</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="A32" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>672</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="D33" s="3" t="s">
+      <c r="A33" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>673</v>
-      </c>
-      <c r="D34" s="3" t="s">
+      <c r="A34" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="3" t="s">
-        <v>674</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>675</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="D35" s="3" t="s">
+      <c r="A35" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="8" t="s">
-        <v>677</v>
-      </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+      <c r="A36" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>678</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>679</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>622</v>
-      </c>
+      <c r="A37" s="8"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" s="8"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A50" s="8"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A47:D49">
+    <sortCondition ref="A47:A49"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5840,7 +6053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B663391-D25B-0045-851E-8A0BB00A0B0A}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>

</xml_diff>

<commit_message>
updated pictures and recruitment info
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brennenwong/dspuci-website-gatsby/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brennenwong/Documents/DSP Website/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF154866-761C-1E49-B765-73E1C24F1936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155AC0FB-A65C-3D4B-AD72-D0877636932A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32140" yWindow="8540" windowWidth="30900" windowHeight="18100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Time Offers 2021" sheetId="15" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="689">
   <si>
     <t>Name</t>
   </si>
@@ -2075,12 +2075,6 @@
     <t>Amanda Nguyen</t>
   </si>
   <si>
-    <t>Business Development Intern</t>
-  </si>
-  <si>
-    <t>Oppti</t>
-  </si>
-  <si>
     <t>Acquisitions Analyst Intern</t>
   </si>
   <si>
@@ -2118,6 +2112,9 @@
   </si>
   <si>
     <t>Risk and Financial Advisor</t>
+  </si>
+  <si>
+    <t>Strathspey Crown Holdings LLC</t>
   </si>
 </sst>
 </file>
@@ -2415,7 +2412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3CD6D6-8A13-7342-A149-99232F890266}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2518,7 +2515,7 @@
         <v>75</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>92</v>
@@ -2535,7 +2532,7 @@
         <v>246</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>622</v>
@@ -2546,7 +2543,7 @@
         <v>93</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>221</v>
@@ -2560,7 +2557,7 @@
         <v>58</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>92</v>
@@ -2596,10 +2593,10 @@
         <v>208</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>622</v>
@@ -2610,10 +2607,10 @@
         <v>209</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>622</v>
@@ -2632,10 +2629,10 @@
         <v>204</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>622</v>
@@ -2654,7 +2651,7 @@
         <v>167</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>188</v>
@@ -5149,8 +5146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D299C4D8-108C-C347-A079-14D1CC67BEF2}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="180" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5336,10 +5333,10 @@
         <v>213</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>622</v>
@@ -5355,13 +5352,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
-        <v>674</v>
+        <v>133</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>676</v>
+        <v>231</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>622</v>
@@ -5369,49 +5366,49 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>133</v>
+        <v>212</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>672</v>
+        <v>267</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>231</v>
+        <v>673</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>673</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="A18" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>203</v>
+        <v>674</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>659</v>
+        <v>97</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>660</v>
+        <v>688</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>622</v>

</xml_diff>

<commit_message>
recruitment flyer, fix fam trees, updated headshots+careers
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Droo\DoT\dspuci-website-gatsby\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED623955-8E52-4EF8-9C4B-4FB0E91360F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E64A96F-B8A2-4AB1-982F-1CBAED2179AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="713">
   <si>
     <t>Name</t>
   </si>
@@ -2177,6 +2177,18 @@
   </si>
   <si>
     <t>Chicago, IL</t>
+  </si>
+  <si>
+    <t>Strategic Finance Intern</t>
+  </si>
+  <si>
+    <t>Ultra Mint Mobile</t>
+  </si>
+  <si>
+    <t>Costa Mesa, US</t>
+  </si>
+  <si>
+    <t>Application Program Analyst Intern</t>
   </si>
 </sst>
 </file>
@@ -5813,10 +5825,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9946A236-302D-42F8-823D-681C430C113E}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5851,132 +5863,156 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>689</v>
+        <v>207</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>687</v>
+        <v>712</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>698</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>699</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>693</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>694</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+    <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>629</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>696</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>697</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>644</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>622</v>
-      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>661</v>
+        <v>629</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>707</v>
+        <v>696</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>708</v>
+        <v>697</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
+      <c r="A12" s="7" t="s">
+        <v>255</v>
+      </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="A13" s="6" t="s">
+        <v>644</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -6011,8 +6047,8 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -6029,14 +6065,14 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+    <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -6047,8 +6083,27 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
bio + career updates
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Droo\DoT\dspuci-website-gatsby\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22531FA-39FC-4582-BC45-D064DE308F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77EF97E-ECA7-46F2-84E0-71E4B7FC920C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Time Offers 2022" sheetId="18" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="719">
   <si>
     <t>Name</t>
   </si>
@@ -2140,12 +2140,6 @@
     <t>New York, US</t>
   </si>
   <si>
-    <t>Summer Associate</t>
-  </si>
-  <si>
-    <t>AlphaSights</t>
-  </si>
-  <si>
     <t>External Audit Intern</t>
   </si>
   <si>
@@ -2195,6 +2189,24 @@
   </si>
   <si>
     <t>Venture Capital</t>
+  </si>
+  <si>
+    <t>Marketing and Sales</t>
+  </si>
+  <si>
+    <t>David Ayala</t>
+  </si>
+  <si>
+    <t>Niagara Bottling</t>
+  </si>
+  <si>
+    <t>Diamond Bar, CA</t>
+  </si>
+  <si>
+    <t>Rotational Finance Analyst</t>
+  </si>
+  <si>
+    <t>Meta</t>
   </si>
 </sst>
 </file>
@@ -2490,10 +2502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92D8086-59A2-468E-9F47-04AE6B52AFA8}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2553,7 +2565,7 @@
         <v>133</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>231</v>
@@ -2572,95 +2584,103 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>704</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>701</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>702</v>
-      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>692</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+    <row r="12" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>703</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>622</v>
-      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>194</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -2675,13 +2695,13 @@
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
+      <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2693,13 +2713,13 @@
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2724,9 +2744,15 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5831,10 +5857,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9946A236-302D-42F8-823D-681C430C113E}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5872,13 +5898,13 @@
         <v>207</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5908,13 +5934,13 @@
         <v>205</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>708</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>709</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5936,10 +5962,10 @@
         <v>210</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>622</v>
@@ -5959,91 +5985,99 @@
         <v>695</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>629</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>696</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>697</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="B10" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>644</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>661</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>706</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B15" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>714</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="D15" s="6" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>712</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>712</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>713</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
@@ -6081,14 +6115,14 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+    <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -6105,17 +6139,23 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+    <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A29" s="8"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added letter to the president
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorin\newest_dspuci_website\dspuci-website-gatsby\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB87B93-FDF2-4CD9-B7BC-63C1AA42991F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2CEF6A-3FD7-4236-9250-5D688FA3771D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7788" yWindow="60" windowWidth="12960" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6025,7 +6025,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6232,167 +6232,167 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>736</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>705</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>718</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>706</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>707</v>
-      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>666</v>
+        <v>705</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>727</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>706</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>748</v>
+        <v>666</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>749</v>
+        <v>726</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>750</v>
+        <v>727</v>
       </c>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>664</v>
+        <v>748</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>323</v>
+        <v>749</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>711</v>
+        <v>750</v>
       </c>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>769</v>
+        <v>664</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>770</v>
+        <v>323</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>771</v>
+        <v>711</v>
       </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>669</v>
+        <v>769</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>716</v>
+        <v>770</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>717</v>
+        <v>771</v>
       </c>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>772</v>
+        <v>669</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>773</v>
+        <v>716</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>771</v>
+        <v>717</v>
       </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>764</v>
+        <v>772</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>206</v>
+        <v>764</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>719</v>
+        <v>767</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>720</v>
+        <v>768</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>761</v>
+        <v>206</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>762</v>
+        <v>719</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>763</v>
+        <v>720</v>
       </c>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>203</v>
+        <v>761</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>728</v>
+        <v>762</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>724</v>
+        <v>728</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="D30" s="3"/>
     </row>

</xml_diff>

<commit_message>
added HR & admin section for careers page
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorin\newest_dspuci_website\dspuci-website-gatsby\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2CEF6A-3FD7-4236-9250-5D688FA3771D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A407AB-DAD2-4CEB-81E0-C7F019D68821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7788" yWindow="60" windowWidth="12960" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="773">
   <si>
     <t>Name</t>
   </si>
@@ -2255,9 +2255,6 @@
   </si>
   <si>
     <t>Riot Games</t>
-  </si>
-  <si>
-    <t>Human Resources</t>
   </si>
   <si>
     <t>Jenny Wu</t>
@@ -6025,7 +6022,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6088,13 +6085,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>756</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>757</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>758</v>
       </c>
       <c r="D5" s="3"/>
     </row>
@@ -6122,25 +6119,25 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>764</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>765</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>766</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>759</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>760</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -6177,22 +6174,22 @@
         <v>213</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>738</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>739</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>454</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D13" s="3"/>
     </row>
@@ -6224,7 +6221,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>735</v>
+        <v>256</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -6244,13 +6241,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>267</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D18" s="3"/>
     </row>
@@ -6290,13 +6287,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>748</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>749</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>750</v>
       </c>
       <c r="D22" s="3"/>
     </row>
@@ -6314,13 +6311,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
+        <v>768</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>769</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>770</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>771</v>
       </c>
       <c r="D24" s="3"/>
     </row>
@@ -6338,25 +6335,25 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
+        <v>771</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>772</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>773</v>
-      </c>
       <c r="C26" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>766</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>767</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>768</v>
       </c>
       <c r="D27" s="3"/>
     </row>
@@ -6374,13 +6371,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
+        <v>760</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>762</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>763</v>
       </c>
       <c r="D29" s="3"/>
     </row>
@@ -6418,13 +6415,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>745</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>746</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>747</v>
       </c>
       <c r="D33" s="3"/>
     </row>
@@ -6456,25 +6453,25 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>645</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>751</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>752</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>753</v>
       </c>
       <c r="D37" s="3"/>
     </row>
@@ -6518,13 +6515,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
+        <v>739</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>740</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>741</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>742</v>
       </c>
       <c r="D41" s="3"/>
     </row>

</xml_diff>

<commit_message>
added full time roles and changed to 39 members
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorin\newest_dspuci_website\dspuci-website-gatsby\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A407AB-DAD2-4CEB-81E0-C7F019D68821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61006B4F-3F0E-4247-9599-308D442A67D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7788" yWindow="60" windowWidth="12960" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7788" yWindow="60" windowWidth="12960" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Time Offers 2022" sheetId="18" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="778">
   <si>
     <t>Name</t>
   </si>
@@ -2369,6 +2369,21 @@
   </si>
   <si>
     <t>Vice President Marketing</t>
+  </si>
+  <si>
+    <t>Consulting Analyst</t>
+  </si>
+  <si>
+    <t>El Monte, CA</t>
+  </si>
+  <si>
+    <t>National Basketball Association (NBA)</t>
+  </si>
+  <si>
+    <t>Junior Product Designer</t>
+  </si>
+  <si>
+    <t>EBizCharge (Century Business Solutions)</t>
   </si>
 </sst>
 </file>
@@ -2664,10 +2679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92D8086-59A2-468E-9F47-04AE6B52AFA8}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2702,174 +2717,194 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>690</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>691</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>694</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>709</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>622</v>
-      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>698</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>695</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>696</v>
-      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>692</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>697</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>622</v>
-      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>194</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="A16" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>775</v>
+      </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="A17" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>776</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>777</v>
+      </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -2881,13 +2916,13 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+      <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2912,9 +2947,15 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6021,7 +6062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9946A236-302D-42F8-823D-681C430C113E}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Alpha Xi website photos and updated those who retook photos
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A30FC4-1021-4968-94C2-A2742F6E1C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90320EB7-2074-4702-AD29-E02C6D42FF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2625" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="2280" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Time Offers 2022" sheetId="18" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="777">
   <si>
     <t>Name</t>
   </si>
@@ -2375,10 +2375,6 @@
   </si>
   <si>
     <t>C3 AI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Associate Software Engineer</t>
   </si>
   <si>
     <t>Founder</t>
@@ -2455,7 +2451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2463,9 +2459,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2684,7 +2677,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2875,12 +2868,12 @@
         <v>427</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>775</v>
+      <c r="B16" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>697</v>
@@ -2894,10 +2887,10 @@
         <v>163</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>776</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>777</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Updated for S'23 recruitment.
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -1,39 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90320EB7-2074-4702-AD29-E02C6D42FF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F139A0A-301B-47F7-AB22-97B20CBFC6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5235" yWindow="2280" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Full Time Offers 2022" sheetId="18" r:id="rId1"/>
-    <sheet name="Internships 2022" sheetId="19" r:id="rId2"/>
-    <sheet name="Full Time Offers 2021" sheetId="15" r:id="rId3"/>
-    <sheet name="Internships 2021" sheetId="16" r:id="rId4"/>
-    <sheet name="Full Time Offers 2020" sheetId="3" r:id="rId5"/>
-    <sheet name="Internships 2020" sheetId="4" r:id="rId6"/>
-    <sheet name="Full Time Offers 2019" sheetId="2" r:id="rId7"/>
-    <sheet name="Internships 2019" sheetId="1" r:id="rId8"/>
-    <sheet name="Full Time Offers 2018" sheetId="5" r:id="rId9"/>
-    <sheet name="Internships 2018" sheetId="6" r:id="rId10"/>
-    <sheet name="Full Time Offers 2017" sheetId="7" r:id="rId11"/>
-    <sheet name="Internships 2017" sheetId="8" r:id="rId12"/>
-    <sheet name="Full Time Offers 2016" sheetId="9" r:id="rId13"/>
-    <sheet name="Internships 2016" sheetId="10" r:id="rId14"/>
-    <sheet name="Full Time Offers 2015" sheetId="11" r:id="rId15"/>
-    <sheet name="Internships 2015" sheetId="12" r:id="rId16"/>
-    <sheet name="Full Time Offers 2014" sheetId="13" r:id="rId17"/>
-    <sheet name="Internships 2014" sheetId="14" r:id="rId18"/>
+    <sheet name="Full Time Offers 2023" sheetId="23" r:id="rId1"/>
+    <sheet name="Internships 2023" sheetId="22" r:id="rId2"/>
+    <sheet name="Full Time Offers 2022" sheetId="18" r:id="rId3"/>
+    <sheet name="Internships 2022" sheetId="19" r:id="rId4"/>
+    <sheet name="Full Time Offers 2021" sheetId="15" r:id="rId5"/>
+    <sheet name="Internships 2021" sheetId="16" r:id="rId6"/>
+    <sheet name="Full Time Offers 2020" sheetId="3" r:id="rId7"/>
+    <sheet name="Internships 2020" sheetId="4" r:id="rId8"/>
+    <sheet name="Full Time Offers 2019" sheetId="2" r:id="rId9"/>
+    <sheet name="Internships 2019" sheetId="1" r:id="rId10"/>
+    <sheet name="Full Time Offers 2018" sheetId="5" r:id="rId11"/>
+    <sheet name="Internships 2018" sheetId="6" r:id="rId12"/>
+    <sheet name="Full Time Offers 2017" sheetId="7" r:id="rId13"/>
+    <sheet name="Internships 2017" sheetId="8" r:id="rId14"/>
+    <sheet name="Full Time Offers 2016" sheetId="9" r:id="rId15"/>
+    <sheet name="Internships 2016" sheetId="10" r:id="rId16"/>
+    <sheet name="Full Time Offers 2015" sheetId="11" r:id="rId17"/>
+    <sheet name="Internships 2015" sheetId="12" r:id="rId18"/>
+    <sheet name="Full Time Offers 2014" sheetId="13" r:id="rId19"/>
+    <sheet name="Internships 2014" sheetId="14" r:id="rId20"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="5">'Internships 2020'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="7">'Internships 2020'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="803">
   <si>
     <t>Name</t>
   </si>
@@ -2134,9 +2136,6 @@
     <t>New York, US</t>
   </si>
   <si>
-    <t>Emerging Talent Program Specialist</t>
-  </si>
-  <si>
     <t>Slack</t>
   </si>
   <si>
@@ -2381,13 +2380,94 @@
   </si>
   <si>
     <t>ApplicantAI</t>
+  </si>
+  <si>
+    <t>Emerson Collective</t>
+  </si>
+  <si>
+    <t>HR Coordinator</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>TTS Analyst</t>
+  </si>
+  <si>
+    <t>Citi</t>
+  </si>
+  <si>
+    <t>Marketing Program Management Intern</t>
+  </si>
+  <si>
+    <t>Duolingo</t>
+  </si>
+  <si>
+    <t>Andrew Doan</t>
+  </si>
+  <si>
+    <t>FLDP Intern</t>
+  </si>
+  <si>
+    <t>Ronica Cheng</t>
+  </si>
+  <si>
+    <t>Asset and Wealth Management SA</t>
+  </si>
+  <si>
+    <t>PMM Intern</t>
+  </si>
+  <si>
+    <t>Consultant</t>
+  </si>
+  <si>
+    <t>HGS Consulting Group</t>
+  </si>
+  <si>
+    <t>Ramped</t>
+  </si>
+  <si>
+    <t>Armanino</t>
+  </si>
+  <si>
+    <t>HCVT</t>
+  </si>
+  <si>
+    <t>UX Researcher Intern</t>
+  </si>
+  <si>
+    <t>Atlassian</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Product Design</t>
+  </si>
+  <si>
+    <t>Anduril</t>
+  </si>
+  <si>
+    <t>L.S. Congleton &amp; Associates</t>
+  </si>
+  <si>
+    <t>Instagram Reels and Engagement Micro-Intern</t>
+  </si>
+  <si>
+    <t>UCI ANTrepreneur Center</t>
+  </si>
+  <si>
+    <t>BTS Analyst</t>
+  </si>
+  <si>
+    <t>Business Technology Solutions Analyst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2430,6 +2510,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2451,7 +2538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2459,6 +2546,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2673,11 +2761,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92D8086-59A2-468E-9F47-04AE6B52AFA8}">
-  <dimension ref="A1:D29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9278A1-054B-49B3-865B-6502A97D8222}">
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2712,203 +2800,167 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>138</v>
+        <v>634</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>770</v>
+        <v>624</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>92</v>
+        <v>625</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>771</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>690</v>
+        <v>788</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>691</v>
+        <v>789</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>624</v>
+        <v>661</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>802</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>625</v>
+        <v>92</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>10</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>133</v>
+        <v>689</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>694</v>
+        <v>687</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>231</v>
+        <v>92</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>146</v>
+        <v>778</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>144</v>
-      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>674</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>628</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>144</v>
-      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>124</v>
+        <v>213</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>656</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>695</v>
+        <v>790</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>696</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>255</v>
-      </c>
+      <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>774</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>427</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>697</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>622</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>775</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>776</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>772</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>773</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
@@ -2917,13 +2969,13 @@
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
+      <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2935,7 +2987,7 @@
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
+      <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -2954,29 +3006,1001 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40:D40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D50">
+    <sortCondition ref="A3:A50"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D48177-9EF2-1D45-80EE-751A8F12EE03}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B2E965-35C6-B34F-B96B-27E9F0AE48DD}">
   <dimension ref="A1:D33"/>
   <sheetViews>
@@ -3429,7 +4453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E244AA19-9506-B144-9EF7-AC6B1CF0AA3F}">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -3672,7 +4696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82BB25F1-A3D3-C841-A6F8-B5EF90040606}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -4203,7 +5227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9031EB02-A95C-D74D-83A4-05A3491E58FE}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -4402,7 +5426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828FE577-CA0A-4842-B5D5-4380510CAFAE}">
   <dimension ref="A1:D29"/>
   <sheetViews>
@@ -4793,7 +5817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E70235-1E9E-6D40-88A1-194511DD28AA}">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -4944,7 +5968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B4F89E-D6CA-6E4F-AF78-0C66C961479F}">
   <dimension ref="A1:D28"/>
   <sheetViews>
@@ -5333,7 +6357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F961FB61-98A8-094A-A8C7-0E7FF49BA3F7}">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -5555,7 +6579,462 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0A3BAF-FDF2-446E-AB48-20EA8F423893}">
+  <dimension ref="A1:D49"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>746</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>791</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>767</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>761</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>751</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>764</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>766</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>717</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>799</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>783</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="6"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="6"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6A3EEF-A80E-B44C-84DA-A35A16B83714}">
   <dimension ref="A1:D38"/>
   <sheetViews>
@@ -6072,12 +7551,302 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92D8086-59A2-468E-9F47-04AE6B52AFA8}">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>777</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>776</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>771</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9946A236-302D-42F8-823D-681C430C113E}">
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6115,13 +7884,13 @@
         <v>207</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -6140,13 +7909,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>751</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>752</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>753</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>754</v>
       </c>
       <c r="D5" s="3"/>
     </row>
@@ -6174,40 +7943,40 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>760</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>761</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>762</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>755</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>756</v>
       </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>472</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>728</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -6229,22 +7998,22 @@
         <v>213</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>734</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>735</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>454</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D13" s="3"/>
     </row>
@@ -6256,10 +8025,10 @@
         <v>220</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>704</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -6270,7 +8039,7 @@
         <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D15" s="3"/>
     </row>
@@ -6287,22 +8056,22 @@
         <v>212</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>721</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>722</v>
       </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>267</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D18" s="3"/>
     </row>
@@ -6316,16 +8085,16 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>703</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>715</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>704</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -6333,22 +8102,22 @@
         <v>666</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>723</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>724</v>
       </c>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>744</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>745</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>746</v>
       </c>
       <c r="D22" s="3"/>
     </row>
@@ -6360,19 +8129,19 @@
         <v>323</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
+        <v>764</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>765</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>766</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>767</v>
       </c>
       <c r="D24" s="3"/>
     </row>
@@ -6381,34 +8150,34 @@
         <v>669</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>713</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>714</v>
       </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
+        <v>767</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>768</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>769</v>
-      </c>
       <c r="C26" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>763</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>764</v>
       </c>
       <c r="D27" s="3"/>
     </row>
@@ -6417,22 +8186,22 @@
         <v>206</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>716</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>717</v>
       </c>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>757</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>758</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>759</v>
       </c>
       <c r="D29" s="3"/>
     </row>
@@ -6441,22 +8210,22 @@
         <v>203</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>725</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>726</v>
       </c>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>109</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D31" s="3"/>
     </row>
@@ -6470,25 +8239,25 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
+        <v>740</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>741</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>742</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>743</v>
       </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>709</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>710</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>711</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>622</v>
@@ -6502,31 +8271,31 @@
         <v>153</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>645</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
+        <v>746</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>747</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>748</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>749</v>
       </c>
       <c r="D37" s="3"/>
     </row>
@@ -6549,10 +8318,10 @@
         <v>202</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>730</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>731</v>
       </c>
       <c r="D39" s="3"/>
     </row>
@@ -6564,19 +8333,19 @@
         <v>426</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>737</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>738</v>
       </c>
       <c r="D41" s="3"/>
     </row>
@@ -6585,18 +8354,18 @@
         <v>661</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -6607,10 +8376,10 @@
         <v>644</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>700</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>701</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>622</v>
@@ -6700,12 +8469,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3CD6D6-8A13-7342-A149-99232F890266}">
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7035,7 +8804,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D299C4D8-108C-C347-A079-14D1CC67BEF2}">
   <dimension ref="A1:D51"/>
   <sheetViews>
@@ -7623,7 +9392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -7939,7 +9708,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B663391-D25B-0045-851E-8A0BB00A0B0A}">
   <dimension ref="A1:G41"/>
   <sheetViews>
@@ -8540,7 +10309,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -8549,7 +10318,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8795,988 +10564,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:D50"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40:D40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="49.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D50">
-    <sortCondition ref="A3:A50"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D48177-9EF2-1D45-80EE-751A8F12EE03}">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated President's Letter and some bro updates
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C15899-612E-42EE-BF0A-977EA65B19DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB7F7A4-55D3-45F2-9B79-4E678751712F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Time Offers 2023" sheetId="23" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="804">
   <si>
     <t>Name</t>
   </si>
@@ -2458,6 +2458,12 @@
   </si>
   <si>
     <t>Finance/Business Operations Intern</t>
+  </si>
+  <si>
+    <t>Full Stack Software Engineer Intern</t>
+  </si>
+  <si>
+    <t>Cubic Transportation Systems</t>
   </si>
 </sst>
 </file>
@@ -2761,8 +2767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9278A1-054B-49B3-865B-6502A97D8222}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6580,8 +6586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0A3BAF-FDF2-446E-AB48-20EA8F423893}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6904,10 +6910,10 @@
         <v>651</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>153</v>
+        <v>802</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>711</v>
+        <v>803</v>
       </c>
       <c r="D28" s="3"/>
     </row>

</xml_diff>

<commit_message>
Updated Part 2 Reqs
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB7F7A4-55D3-45F2-9B79-4E678751712F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F7D9E7-0CE7-49DE-8BB9-6BD3C6095DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Time Offers 2023" sheetId="23" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="803">
   <si>
     <t>Name</t>
   </si>
@@ -2373,18 +2373,6 @@
     <t>C3 AI</t>
   </si>
   <si>
-    <t>Founder</t>
-  </si>
-  <si>
-    <t>ApplicantAI</t>
-  </si>
-  <si>
-    <t>Emerson Collective</t>
-  </si>
-  <si>
-    <t>HR Coordinator</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
@@ -2464,6 +2452,15 @@
   </si>
   <si>
     <t>Cubic Transportation Systems</t>
+  </si>
+  <si>
+    <t>Data Scientist</t>
+  </si>
+  <si>
+    <t>NBA</t>
+  </si>
+  <si>
+    <t>Project Coordinator</t>
   </si>
 </sst>
 </file>
@@ -2820,10 +2817,10 @@
         <v>202</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>17</v>
@@ -2834,7 +2831,7 @@
         <v>661</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>92</v>
@@ -2848,7 +2845,7 @@
         <v>207</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>92</v>
@@ -2868,7 +2865,7 @@
         <v>92</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2876,7 +2873,7 @@
         <v>629</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>92</v>
@@ -2923,7 +2920,7 @@
         <v>656</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>244</v>
@@ -6586,7 +6583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0A3BAF-FDF2-446E-AB48-20EA8F423893}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -6628,7 +6625,7 @@
         <v>472</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="D3" s="3"/>
     </row>
@@ -6657,7 +6654,7 @@
         <v>740</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>186</v>
@@ -6672,7 +6669,7 @@
         <v>398</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -6684,7 +6681,7 @@
         <v>86</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -6693,10 +6690,10 @@
         <v>766</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -6705,7 +6702,7 @@
         <v>759</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>760</v>
@@ -6714,10 +6711,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>343</v>
@@ -6805,10 +6802,10 @@
         <v>749</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="D19" s="3"/>
     </row>
@@ -6841,7 +6838,7 @@
         <v>717</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>188</v>
@@ -6853,10 +6850,10 @@
         <v>664</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -6869,13 +6866,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="D25" s="3"/>
     </row>
@@ -6896,13 +6893,13 @@
         <v>708</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -6910,10 +6907,10 @@
         <v>651</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="D28" s="3"/>
     </row>
@@ -7558,8 +7555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92D8086-59A2-468E-9F47-04AE6B52AFA8}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7633,10 +7630,10 @@
         <v>133</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>776</v>
+        <v>802</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>775</v>
+        <v>231</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>146</v>
@@ -7755,10 +7752,10 @@
         <v>163</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>773</v>
+        <v>800</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>774</v>
+        <v>801</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>7</v>
@@ -7949,7 +7946,7 @@
         <v>759</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>760</v>

</xml_diff>

<commit_message>
Update before Alpha Omicrons
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F7D9E7-0CE7-49DE-8BB9-6BD3C6095DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EC292A-77A4-427D-9D6D-471046407C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Time Offers 2023" sheetId="23" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="810">
   <si>
     <t>Name</t>
   </si>
@@ -2461,6 +2461,27 @@
   </si>
   <si>
     <t>Project Coordinator</t>
+  </si>
+  <si>
+    <t>HR Specialist</t>
+  </si>
+  <si>
+    <t>Asset Management</t>
+  </si>
+  <si>
+    <t>VLA Business Associate</t>
+  </si>
+  <si>
+    <t>FDP Intern</t>
+  </si>
+  <si>
+    <t>Data Analytics Intern</t>
+  </si>
+  <si>
+    <t>Diana Huynh</t>
+  </si>
+  <si>
+    <t>General Atomics Aeronautical Systems, Inc</t>
   </si>
 </sst>
 </file>
@@ -2762,10 +2783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9278A1-054B-49B3-865B-6502A97D8222}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2905,65 +2926,83 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>721</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>785</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>773</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="A16" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
+      <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
+      <c r="A19" s="4"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -2975,13 +3014,13 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
+      <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
+      <c r="A22" s="4"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -3006,9 +3045,15 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6581,10 +6626,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0A3BAF-FDF2-446E-AB48-20EA8F423893}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C34" sqref="C33:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6726,7 +6771,7 @@
         <v>751</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>754</v>
+        <v>806</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>755</v>
@@ -6889,35 +6934,41 @@
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>708</v>
+      <c r="A27" s="3" t="s">
+        <v>808</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>788</v>
+        <v>807</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>789</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>790</v>
-      </c>
+        <v>809</v>
+      </c>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>651</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>798</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>799</v>
       </c>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -6926,11 +6977,11 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
@@ -6939,16 +6990,16 @@
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
+      <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="4"/>
+      <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
@@ -6993,13 +7044,13 @@
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="6"/>
+      <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
+      <c r="A45" s="6"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -7017,16 +7068,22 @@
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="6"/>
+      <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
+      <c r="A49" s="6"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7555,8 +7612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92D8086-59A2-468E-9F47-04AE6B52AFA8}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Final Update for AO
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EC292A-77A4-427D-9D6D-471046407C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE95F0B5-E1A4-4F45-8A65-FCBD3DD57A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22275" yWindow="405" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Time Offers 2023" sheetId="23" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="812">
   <si>
     <t>Name</t>
   </si>
@@ -2400,9 +2400,6 @@
     <t>Asset and Wealth Management SA</t>
   </si>
   <si>
-    <t>PMM Intern</t>
-  </si>
-  <si>
     <t>Consultant</t>
   </si>
   <si>
@@ -2433,12 +2430,6 @@
     <t>L.S. Congleton &amp; Associates</t>
   </si>
   <si>
-    <t>Instagram Reels and Engagement Micro-Intern</t>
-  </si>
-  <si>
-    <t>UCI ANTrepreneur Center</t>
-  </si>
-  <si>
     <t>Business Technology Solutions Analyst</t>
   </si>
   <si>
@@ -2472,9 +2463,6 @@
     <t>VLA Business Associate</t>
   </si>
   <si>
-    <t>FDP Intern</t>
-  </si>
-  <si>
     <t>Data Analytics Intern</t>
   </si>
   <si>
@@ -2482,6 +2470,24 @@
   </si>
   <si>
     <t>General Atomics Aeronautical Systems, Inc</t>
+  </si>
+  <si>
+    <t>Digital Marketing &amp; Sales Strategy Intern</t>
+  </si>
+  <si>
+    <t>SoKit Beauty</t>
+  </si>
+  <si>
+    <t>Finance Development Program (FDP) Intern</t>
+  </si>
+  <si>
+    <t>Business Planning Intern</t>
+  </si>
+  <si>
+    <t>Notion Campus Leader</t>
+  </si>
+  <si>
+    <t>Notion</t>
   </si>
 </sst>
 </file>
@@ -2785,7 +2791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9278A1-054B-49B3-865B-6502A97D8222}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -2838,10 +2844,10 @@
         <v>202</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>783</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>784</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>17</v>
@@ -2852,7 +2858,7 @@
         <v>661</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>92</v>
@@ -2866,7 +2872,7 @@
         <v>207</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>92</v>
@@ -2894,7 +2900,7 @@
         <v>629</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>92</v>
@@ -2930,7 +2936,7 @@
         <v>210</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>186</v>
@@ -2950,7 +2956,7 @@
         <v>212</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>721</v>
@@ -2972,7 +2978,7 @@
         <v>203</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>149</v>
@@ -2989,7 +2995,7 @@
         <v>656</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>244</v>
@@ -6628,8 +6634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0A3BAF-FDF2-446E-AB48-20EA8F423893}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C33:C34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6670,7 +6676,7 @@
         <v>472</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D3" s="3"/>
     </row>
@@ -6714,7 +6720,7 @@
         <v>398</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -6726,7 +6732,7 @@
         <v>86</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -6747,7 +6753,7 @@
         <v>759</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>760</v>
@@ -6771,7 +6777,7 @@
         <v>751</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>755</v>
@@ -6871,19 +6877,19 @@
         <v>669</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>712</v>
+        <v>810</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>713</v>
+        <v>811</v>
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>717</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>782</v>
+        <v>809</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>188</v>
@@ -6895,10 +6901,10 @@
         <v>664</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>793</v>
+        <v>806</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>794</v>
+        <v>807</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -6914,10 +6920,10 @@
         <v>778</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D25" s="3"/>
     </row>
@@ -6935,13 +6941,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="D27" s="3"/>
     </row>
@@ -6950,13 +6956,13 @@
         <v>708</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>788</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>789</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -6964,10 +6970,10 @@
         <v>651</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="D29" s="3"/>
     </row>
@@ -7687,7 +7693,7 @@
         <v>133</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>231</v>
@@ -7809,10 +7815,10 @@
         <v>163</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>7</v>
@@ -8003,7 +8009,7 @@
         <v>759</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>760</v>

</xml_diff>

<commit_message>
Last Summer/Fall Updates by Kevin
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE95F0B5-E1A4-4F45-8A65-FCBD3DD57A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ED1F5B-98C1-4A03-99E9-C6E7B1D827B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22275" yWindow="405" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6960" yWindow="3000" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Time Offers 2023" sheetId="23" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1837" uniqueCount="841">
   <si>
     <t>Name</t>
   </si>
@@ -2397,9 +2397,6 @@
     <t>Ronica Cheng</t>
   </si>
   <si>
-    <t>Asset and Wealth Management SA</t>
-  </si>
-  <si>
     <t>Consultant</t>
   </si>
   <si>
@@ -2488,13 +2485,103 @@
   </si>
   <si>
     <t>Notion</t>
+  </si>
+  <si>
+    <t>Sales Intern</t>
+  </si>
+  <si>
+    <t>Mirsab Mirza</t>
+  </si>
+  <si>
+    <t>LA Rams</t>
+  </si>
+  <si>
+    <t>Jacob Won</t>
+  </si>
+  <si>
+    <t>Alpha Omega Group</t>
+  </si>
+  <si>
+    <t>Asset and Wealth Management Summer Analyst</t>
+  </si>
+  <si>
+    <t>J.P. Morgan Private Bank</t>
+  </si>
+  <si>
+    <t>Nithin Senthil</t>
+  </si>
+  <si>
+    <t>LoginID</t>
+  </si>
+  <si>
+    <t>Aadi Mehta</t>
+  </si>
+  <si>
+    <t>SMUD</t>
+  </si>
+  <si>
+    <t>SAP System Analyst Intern</t>
+  </si>
+  <si>
+    <t>Tommy Wunsch</t>
+  </si>
+  <si>
+    <t>Studio Store Intern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOX Entertainment </t>
+  </si>
+  <si>
+    <t>Ishan Malik</t>
+  </si>
+  <si>
+    <t>Operations Intern</t>
+  </si>
+  <si>
+    <t>Siemens</t>
+  </si>
+  <si>
+    <t>Jessica Lin</t>
+  </si>
+  <si>
+    <t>R&amp;F Mart</t>
+  </si>
+  <si>
+    <t>Juliana Lee</t>
+  </si>
+  <si>
+    <t>Niche Street</t>
+  </si>
+  <si>
+    <t>Social Media Marketing Manager</t>
+  </si>
+  <si>
+    <t>Communications and Advocacy Intern</t>
+  </si>
+  <si>
+    <t>LCLAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julitza Alvarez </t>
+  </si>
+  <si>
+    <t>Collin Na</t>
+  </si>
+  <si>
+    <t>The Reserve Investments</t>
+  </si>
+  <si>
+    <t>Brennan Kim</t>
+  </si>
+  <si>
+    <t>Consumer Insights Research Intern</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2544,6 +2631,18 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2565,7 +2664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2574,6 +2673,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2844,10 +2948,10 @@
         <v>202</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>782</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>783</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>17</v>
@@ -2858,7 +2962,7 @@
         <v>661</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>92</v>
@@ -2872,7 +2976,7 @@
         <v>207</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>92</v>
@@ -2900,7 +3004,7 @@
         <v>629</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>92</v>
@@ -2936,7 +3040,7 @@
         <v>210</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>186</v>
@@ -2956,7 +3060,7 @@
         <v>212</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>721</v>
@@ -2978,7 +3082,7 @@
         <v>203</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>149</v>
@@ -2995,7 +3099,7 @@
         <v>656</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>244</v>
@@ -6632,10 +6736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0A3BAF-FDF2-446E-AB48-20EA8F423893}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6676,7 +6780,7 @@
         <v>472</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D3" s="3"/>
     </row>
@@ -6705,364 +6809,430 @@
         <v>740</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>781</v>
+        <v>816</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>186</v>
+        <v>817</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>735</v>
+        <v>837</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>398</v>
+        <v>52</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>785</v>
+        <v>838</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>86</v>
+        <v>398</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>766</v>
+        <v>738</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>774</v>
+        <v>86</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>775</v>
+        <v>785</v>
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>759</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>794</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>760</v>
+        <v>814</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>815</v>
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>780</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>779</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>343</v>
+        <v>829</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>830</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>766</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>751</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>808</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B15" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>755</v>
       </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>732</v>
-      </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>743</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>744</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>745</v>
-      </c>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>644</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>702</v>
+        <v>836</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>714</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>703</v>
+        <v>834</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>835</v>
       </c>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>749</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>776</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>777</v>
-      </c>
+      <c r="A19" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>763</v>
+        <v>743</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>764</v>
+        <v>811</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>765</v>
+        <v>229</v>
       </c>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>669</v>
+      <c r="A21" s="3" t="s">
+        <v>644</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>810</v>
+        <v>334</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>811</v>
+        <v>188</v>
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>717</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>809</v>
+        <v>839</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>840</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>188</v>
+        <v>825</v>
       </c>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>664</v>
+        <v>702</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>806</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>807</v>
-      </c>
+        <v>714</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="A24" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>776</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>777</v>
+      </c>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>778</v>
+        <v>763</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>793</v>
+        <v>764</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>790</v>
+        <v>765</v>
       </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
+        <v>831</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>717</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>812</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>823</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>824</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>825</v>
+      </c>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>820</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>821</v>
+      </c>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
         <v>648</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>706</v>
       </c>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>804</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>803</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>805</v>
-      </c>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>826</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>708</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B38" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>787</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>788</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>818</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>819</v>
+      </c>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
         <v>651</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B40" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>795</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>796</v>
-      </c>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
+      <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
+      <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-    </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="6"/>
+      <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
+      <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -7071,7 +7241,7 @@
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
@@ -7080,7 +7250,7 @@
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="6"/>
+      <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -7090,6 +7260,72 @@
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="6"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="6"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7693,7 +7929,7 @@
         <v>133</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>231</v>
@@ -7815,10 +8051,10 @@
         <v>163</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>797</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>798</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>7</v>
@@ -8009,7 +8245,7 @@
         <v>759</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>760</v>

</xml_diff>